<commit_message>
fixed problem with small files
</commit_message>
<xml_diff>
--- a/01-ouput-files/log-files/CONSOLIDATED.xlsx
+++ b/01-ouput-files/log-files/CONSOLIDATED.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="B9" s="2">
-        <v>44364.54704801041</v>
+        <v>44375.90949464121</v>
       </c>
       <c r="C9">
         <v>108</v>
@@ -869,7 +869,7 @@
         </is>
       </c>
       <c r="B10" s="2">
-        <v>44364.54712204514</v>
+        <v>44375.90957033912</v>
       </c>
       <c r="C10">
         <v>284</v>
@@ -921,7 +921,7 @@
         </is>
       </c>
       <c r="B11" s="2">
-        <v>44364.54722295486</v>
+        <v>44375.90967922685</v>
       </c>
       <c r="C11">
         <v>481</v>
@@ -973,7 +973,7 @@
         </is>
       </c>
       <c r="B12" s="2">
-        <v>44364.54726667361</v>
+        <v>44375.90972654746</v>
       </c>
       <c r="C12">
         <v>93</v>
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="B13" s="2">
-        <v>44364.54730291898</v>
+        <v>44375.90976891898</v>
       </c>
       <c r="C13">
         <v>229</v>
@@ -1068,6 +1068,22 @@
       </c>
       <c r="P13">
         <v>0.09606986899563319</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ytube-transcripts-text---rZkdPXP6H4.txt</t>
+        </is>
+      </c>
+      <c r="B14" s="2">
+        <v>44375.90801329167</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue with filtering
</commit_message>
<xml_diff>
--- a/01-ouput-files/log-files/CONSOLIDATED.xlsx
+++ b/01-ouput-files/log-files/CONSOLIDATED.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1077,13 +1077,77 @@
         </is>
       </c>
       <c r="B14" s="2">
-        <v>44375.90801329167</v>
+        <v>44382.88801283449</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
         <v>34</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ytube-transcripts-text--00QUYoZHnH8.txt</t>
+        </is>
+      </c>
+      <c r="B15" s="2">
+        <v>44382.88804535648</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ytube-transcripts-text--0H5QZvOqlJM.txt</t>
+        </is>
+      </c>
+      <c r="B16" s="2">
+        <v>44382.88807880093</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ytube-transcripts-text--24R8JObNNQ4.txt</t>
+        </is>
+      </c>
+      <c r="B17" s="2">
+        <v>44382.88811206944</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ytube-transcripts-text--3HJj85K_7MQ.txt</t>
+        </is>
+      </c>
+      <c r="B18" s="2">
+        <v>44382.88814605093</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>